<commit_message>
Updated parsed output of iHawk test cases
</commit_message>
<xml_diff>
--- a/output/231120_123524_93d5c35_macOS/7_NT_A_2 – iHawk mit 16 Kanäle (Tuning ohne Interrupt-Moderation)/campaign/7_NT_A_2 – iHawk mit 16 Kanäle (Tuning ohne Interrupt-Moderation)_campaign_overview.xlsx
+++ b/output/231120_123524_93d5c35_macOS/7_NT_A_2 – iHawk mit 16 Kanäle (Tuning ohne Interrupt-Moderation)/campaign/7_NT_A_2 – iHawk mit 16 Kanäle (Tuning ohne Interrupt-Moderation)_campaign_overview.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bornkessel/Developer/testresults/output/231120_123524_93d5c35_macOS/7_NT_A_2 – iHawk mit 16 Kanäle (Tuning ohne Interrupt-Moderation)/campaign/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{966837FD-A443-F946-AF80-F7F76C665C94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FADC232-1D5D-1640-A4F7-18CF39BA4B46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4300" yWindow="780" windowWidth="29900" windowHeight="19900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4300" yWindow="780" windowWidth="29900" windowHeight="19820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="355" uniqueCount="60">
   <si>
     <t>Duration (s)</t>
   </si>
@@ -210,17 +210,22 @@
   </si>
   <si>
     <t>814807_175035_131123</t>
+  </si>
+  <si>
+    <t>Spalte1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="0.000%"/>
+    <numFmt numFmtId="167" formatCode="0.00000000000000000000%"/>
+    <numFmt numFmtId="200" formatCode="0.000000000000000000000%"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -246,13 +251,26 @@
       <sz val="11"/>
       <name val="Consolas"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -279,10 +297,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -292,11 +311,45 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="200" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Prozent" xfId="1" builtinId="5"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color auto="1"/>
+        <name val="Consolas"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -310,9 +363,9 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:W47">
-  <autoFilter ref="A1:W47" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
-  <tableColumns count="23">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:X47">
+  <autoFilter ref="A1:X47" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+  <tableColumns count="24">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Duration (s)"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Method"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Test-ID"/>
@@ -327,6 +380,9 @@
     <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="Location"/>
     <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="Status"/>
     <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="Losses [total]"/>
+    <tableColumn id="24" xr3:uid="{9E341BFB-73CB-5F46-836D-480A8C9E2879}" name="Spalte1" dataDxfId="0">
+      <calculatedColumnFormula>Table1[[#This Row],[Losses '[ratio'](%)]]*1000000</calculatedColumnFormula>
+    </tableColumn>
     <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="Losses [ratio](%)"/>
     <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="Losses [location]"/>
     <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="Pakets [total]"/>
@@ -626,23 +682,31 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:W52"/>
+  <dimension ref="A1:X55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="Q51" sqref="Q51"/>
+    <sheetView tabSelected="1" topLeftCell="D18" workbookViewId="0">
+      <selection activeCell="P52" sqref="P52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="1" max="1" width="9" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="22" customWidth="1"/>
     <col min="4" max="6" width="13" customWidth="1"/>
+    <col min="7" max="9" width="9" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="15" customWidth="1"/>
-    <col min="16" max="16" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="25.33203125" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="15" customWidth="1"/>
+    <col min="18" max="18" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="20" max="21" width="9" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="12.1640625" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="20" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -686,34 +750,37 @@
         <v>13</v>
       </c>
       <c r="O1" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="P1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>7199.5882879999999</v>
       </c>
@@ -756,31 +823,35 @@
       <c r="N2" s="5">
         <v>0</v>
       </c>
-      <c r="O2" s="6">
-        <v>0</v>
-      </c>
-      <c r="P2" s="3"/>
-      <c r="Q2" s="5">
+      <c r="O2" s="5">
+        <f>Table1[[#This Row],[Losses '[ratio'](%)]]*1000000</f>
+        <v>0</v>
+      </c>
+      <c r="P2" s="6">
+        <v>0</v>
+      </c>
+      <c r="Q2" s="3"/>
+      <c r="R2" s="5">
         <v>291939524</v>
-      </c>
-      <c r="R2" s="5">
-        <v>40549</v>
       </c>
       <c r="S2" s="5">
         <v>40549</v>
       </c>
-      <c r="T2" s="2">
+      <c r="T2" s="5">
+        <v>40549</v>
+      </c>
+      <c r="U2" s="2">
         <v>25.951360000000001</v>
       </c>
-      <c r="U2" s="2">
+      <c r="V2" s="2">
         <v>39.575823999999997</v>
       </c>
-      <c r="V2" s="5">
+      <c r="W2" s="5">
         <v>-1707068586</v>
       </c>
-      <c r="W2" s="3"/>
-    </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X2" s="3"/>
+    </row>
+    <row r="3" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>7199.5829620000004</v>
       </c>
@@ -823,31 +894,35 @@
       <c r="N3" s="5">
         <v>0</v>
       </c>
-      <c r="O3" s="6">
-        <v>0</v>
-      </c>
-      <c r="P3" s="3"/>
-      <c r="Q3" s="5">
+      <c r="O3" s="5">
+        <f>Table1[[#This Row],[Losses '[ratio'](%)]]*1000000</f>
+        <v>0</v>
+      </c>
+      <c r="P3" s="6">
+        <v>0</v>
+      </c>
+      <c r="Q3" s="3"/>
+      <c r="R3" s="5">
         <v>291375660</v>
-      </c>
-      <c r="R3" s="5">
-        <v>40471</v>
       </c>
       <c r="S3" s="5">
         <v>40471</v>
       </c>
-      <c r="T3" s="2">
+      <c r="T3" s="5">
+        <v>40471</v>
+      </c>
+      <c r="U3" s="2">
         <v>25.901440000000001</v>
       </c>
-      <c r="U3" s="2">
+      <c r="V3" s="2">
         <v>39.499696</v>
       </c>
-      <c r="V3" s="5">
+      <c r="W3" s="5">
         <v>-1706506859</v>
       </c>
-      <c r="W3" s="3"/>
-    </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X3" s="3"/>
+    </row>
+    <row r="4" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>7199.1868919999997</v>
       </c>
@@ -890,31 +965,35 @@
       <c r="N4" s="5">
         <v>0</v>
       </c>
-      <c r="O4" s="6">
-        <v>0</v>
-      </c>
-      <c r="P4" s="3"/>
-      <c r="Q4" s="5">
+      <c r="O4" s="5">
+        <f>Table1[[#This Row],[Losses '[ratio'](%)]]*1000000</f>
+        <v>0</v>
+      </c>
+      <c r="P4" s="6">
+        <v>0</v>
+      </c>
+      <c r="Q4" s="3"/>
+      <c r="R4" s="5">
         <v>1096469811</v>
-      </c>
-      <c r="R4" s="5">
-        <v>152304</v>
       </c>
       <c r="S4" s="5">
         <v>152304</v>
       </c>
-      <c r="T4" s="2">
+      <c r="T4" s="5">
+        <v>152304</v>
+      </c>
+      <c r="U4" s="2">
         <v>97.474559999999997</v>
       </c>
-      <c r="U4" s="2">
+      <c r="V4" s="2">
         <v>148.64870400000001</v>
       </c>
-      <c r="V4" s="5">
+      <c r="W4" s="5">
         <v>1783215909</v>
       </c>
-      <c r="W4" s="3"/>
-    </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X4" s="3"/>
+    </row>
+    <row r="5" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>7199.5879880000002</v>
       </c>
@@ -957,31 +1036,35 @@
       <c r="N5" s="5">
         <v>0</v>
       </c>
-      <c r="O5" s="6">
-        <v>0</v>
-      </c>
-      <c r="P5" s="3"/>
-      <c r="Q5" s="5">
+      <c r="O5" s="5">
+        <f>Table1[[#This Row],[Losses '[ratio'](%)]]*1000000</f>
+        <v>0</v>
+      </c>
+      <c r="P5" s="6">
+        <v>0</v>
+      </c>
+      <c r="Q5" s="3"/>
+      <c r="R5" s="5">
         <v>294009558</v>
-      </c>
-      <c r="R5" s="5">
-        <v>40836</v>
       </c>
       <c r="S5" s="5">
         <v>40836</v>
       </c>
-      <c r="T5" s="2">
+      <c r="T5" s="5">
+        <v>40836</v>
+      </c>
+      <c r="U5" s="2">
         <v>26.13504</v>
       </c>
-      <c r="U5" s="2">
+      <c r="V5" s="2">
         <v>39.855936</v>
       </c>
-      <c r="V5" s="5">
+      <c r="W5" s="5">
         <v>-1709138719</v>
       </c>
-      <c r="W5" s="3"/>
-    </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X5" s="3"/>
+    </row>
+    <row r="6" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>7199.5818289999997</v>
       </c>
@@ -1024,31 +1107,35 @@
       <c r="N6" s="5">
         <v>0</v>
       </c>
-      <c r="O6" s="6">
-        <v>0</v>
-      </c>
-      <c r="P6" s="3"/>
-      <c r="Q6" s="5">
+      <c r="O6" s="5">
+        <f>Table1[[#This Row],[Losses '[ratio'](%)]]*1000000</f>
+        <v>0</v>
+      </c>
+      <c r="P6" s="6">
+        <v>0</v>
+      </c>
+      <c r="Q6" s="3"/>
+      <c r="R6" s="5">
         <v>292225288</v>
-      </c>
-      <c r="R6" s="5">
-        <v>40589</v>
       </c>
       <c r="S6" s="5">
         <v>40589</v>
       </c>
-      <c r="T6" s="2">
+      <c r="T6" s="5">
+        <v>40589</v>
+      </c>
+      <c r="U6" s="2">
         <v>25.976959999999998</v>
       </c>
-      <c r="U6" s="2">
+      <c r="V6" s="2">
         <v>39.614863999999997</v>
       </c>
-      <c r="V6" s="5">
+      <c r="W6" s="5">
         <v>-1707356931</v>
       </c>
-      <c r="W6" s="3"/>
-    </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X6" s="3"/>
+    </row>
+    <row r="7" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <v>7199.1884579999996</v>
       </c>
@@ -1091,31 +1178,35 @@
       <c r="N7" s="5">
         <v>0</v>
       </c>
-      <c r="O7" s="6">
-        <v>0</v>
-      </c>
-      <c r="P7" s="3"/>
-      <c r="Q7" s="5">
+      <c r="O7" s="5">
+        <f>Table1[[#This Row],[Losses '[ratio'](%)]]*1000000</f>
+        <v>0</v>
+      </c>
+      <c r="P7" s="6">
+        <v>0</v>
+      </c>
+      <c r="Q7" s="3"/>
+      <c r="R7" s="5">
         <v>1140487478</v>
-      </c>
-      <c r="R7" s="5">
-        <v>158418</v>
       </c>
       <c r="S7" s="5">
         <v>158418</v>
       </c>
-      <c r="T7" s="2">
+      <c r="T7" s="5">
+        <v>158418</v>
+      </c>
+      <c r="U7" s="2">
         <v>101.38751999999999</v>
       </c>
-      <c r="U7" s="2">
+      <c r="V7" s="2">
         <v>154.61596800000001</v>
       </c>
-      <c r="V7" s="5">
+      <c r="W7" s="5">
         <v>1739199309</v>
       </c>
-      <c r="W7" s="3"/>
-    </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X7" s="3"/>
+    </row>
+    <row r="8" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <v>7199.8864370000001</v>
       </c>
@@ -1158,31 +1249,35 @@
       <c r="N8" s="5">
         <v>0</v>
       </c>
-      <c r="O8" s="6">
-        <v>0</v>
-      </c>
-      <c r="P8" s="3"/>
-      <c r="Q8" s="5">
+      <c r="O8" s="5">
+        <f>Table1[[#This Row],[Losses '[ratio'](%)]]*1000000</f>
+        <v>0</v>
+      </c>
+      <c r="P8" s="6">
+        <v>0</v>
+      </c>
+      <c r="Q8" s="3"/>
+      <c r="R8" s="5">
         <v>1133563690</v>
-      </c>
-      <c r="R8" s="5">
-        <v>157441</v>
       </c>
       <c r="S8" s="5">
         <v>157441</v>
       </c>
-      <c r="T8" s="2">
+      <c r="T8" s="5">
+        <v>157441</v>
+      </c>
+      <c r="U8" s="2">
         <v>100.76224000000001</v>
       </c>
-      <c r="U8" s="2">
+      <c r="V8" s="2">
         <v>153.66241600000001</v>
       </c>
-      <c r="V8" s="5">
+      <c r="W8" s="5">
         <v>1746402219</v>
       </c>
-      <c r="W8" s="3"/>
-    </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X8" s="3"/>
+    </row>
+    <row r="9" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
         <v>7199.2426530000002</v>
       </c>
@@ -1225,31 +1320,35 @@
       <c r="N9" s="5">
         <v>0</v>
       </c>
-      <c r="O9" s="6">
-        <v>0</v>
-      </c>
-      <c r="P9" s="3"/>
-      <c r="Q9" s="5">
+      <c r="O9" s="5">
+        <f>Table1[[#This Row],[Losses '[ratio'](%)]]*1000000</f>
+        <v>0</v>
+      </c>
+      <c r="P9" s="6">
+        <v>0</v>
+      </c>
+      <c r="Q9" s="3"/>
+      <c r="R9" s="5">
         <v>793914983</v>
-      </c>
-      <c r="R9" s="5">
-        <v>110277</v>
       </c>
       <c r="S9" s="5">
         <v>110277</v>
       </c>
-      <c r="T9" s="2">
+      <c r="T9" s="5">
+        <v>110277</v>
+      </c>
+      <c r="U9" s="2">
         <v>70.577280000000002</v>
       </c>
-      <c r="U9" s="2">
+      <c r="V9" s="2">
         <v>107.630352</v>
       </c>
-      <c r="V9" s="5">
+      <c r="W9" s="5">
         <v>2085790016</v>
       </c>
-      <c r="W9" s="3"/>
-    </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X9" s="3"/>
+    </row>
+    <row r="10" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
         <v>7199.5840790000002</v>
       </c>
@@ -1292,31 +1391,35 @@
       <c r="N10" s="5">
         <v>0</v>
       </c>
-      <c r="O10" s="6">
-        <v>0</v>
-      </c>
-      <c r="P10" s="3"/>
-      <c r="Q10" s="5">
+      <c r="O10" s="5">
+        <f>Table1[[#This Row],[Losses '[ratio'](%)]]*1000000</f>
+        <v>0</v>
+      </c>
+      <c r="P10" s="6">
+        <v>0</v>
+      </c>
+      <c r="Q10" s="3"/>
+      <c r="R10" s="5">
         <v>298161224</v>
-      </c>
-      <c r="R10" s="5">
-        <v>41413</v>
       </c>
       <c r="S10" s="5">
         <v>41413</v>
       </c>
-      <c r="T10" s="2">
+      <c r="T10" s="5">
+        <v>41413</v>
+      </c>
+      <c r="U10" s="2">
         <v>26.50432</v>
       </c>
-      <c r="U10" s="2">
+      <c r="V10" s="2">
         <v>40.419088000000002</v>
       </c>
-      <c r="V10" s="5">
+      <c r="W10" s="5">
         <v>-1713291908</v>
       </c>
-      <c r="W10" s="3"/>
-    </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X10" s="3"/>
+    </row>
+    <row r="11" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
         <v>7199.332195</v>
       </c>
@@ -1359,31 +1462,35 @@
       <c r="N11" s="5">
         <v>0</v>
       </c>
-      <c r="O11" s="6">
-        <v>0</v>
-      </c>
-      <c r="P11" s="3"/>
-      <c r="Q11" s="5">
+      <c r="O11" s="5">
+        <f>Table1[[#This Row],[Losses '[ratio'](%)]]*1000000</f>
+        <v>0</v>
+      </c>
+      <c r="P11" s="6">
+        <v>0</v>
+      </c>
+      <c r="Q11" s="3"/>
+      <c r="R11" s="5">
         <v>827144793</v>
-      </c>
-      <c r="R11" s="5">
-        <v>114891</v>
       </c>
       <c r="S11" s="5">
         <v>114891</v>
       </c>
-      <c r="T11" s="2">
+      <c r="T11" s="5">
+        <v>114891</v>
+      </c>
+      <c r="U11" s="2">
         <v>73.530240000000006</v>
       </c>
-      <c r="U11" s="2">
+      <c r="V11" s="2">
         <v>112.133616</v>
       </c>
-      <c r="V11" s="5">
+      <c r="W11" s="5">
         <v>2052596355</v>
       </c>
-      <c r="W11" s="3"/>
-    </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X11" s="3"/>
+    </row>
+    <row r="12" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
         <v>7199.5864199999996</v>
       </c>
@@ -1426,31 +1533,35 @@
       <c r="N12" s="5">
         <v>0</v>
       </c>
-      <c r="O12" s="6">
-        <v>0</v>
-      </c>
-      <c r="P12" s="3"/>
-      <c r="Q12" s="5">
+      <c r="O12" s="5">
+        <f>Table1[[#This Row],[Losses '[ratio'](%)]]*1000000</f>
+        <v>0</v>
+      </c>
+      <c r="P12" s="6">
+        <v>0</v>
+      </c>
+      <c r="Q12" s="3"/>
+      <c r="R12" s="5">
         <v>291078720</v>
-      </c>
-      <c r="R12" s="5">
-        <v>40429</v>
       </c>
       <c r="S12" s="5">
         <v>40429</v>
       </c>
-      <c r="T12" s="2">
+      <c r="T12" s="5">
+        <v>40429</v>
+      </c>
+      <c r="U12" s="2">
         <v>25.874559999999999</v>
       </c>
-      <c r="U12" s="2">
+      <c r="V12" s="2">
         <v>39.458703999999997</v>
       </c>
-      <c r="V12" s="5">
+      <c r="W12" s="5">
         <v>-1706208539</v>
       </c>
-      <c r="W12" s="3"/>
-    </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X12" s="3"/>
+    </row>
+    <row r="13" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
         <v>7199.887643</v>
       </c>
@@ -1493,31 +1604,35 @@
       <c r="N13" s="5">
         <v>0</v>
       </c>
-      <c r="O13" s="6">
-        <v>0</v>
-      </c>
-      <c r="P13" s="3"/>
-      <c r="Q13" s="5">
+      <c r="O13" s="5">
+        <f>Table1[[#This Row],[Losses '[ratio'](%)]]*1000000</f>
+        <v>0</v>
+      </c>
+      <c r="P13" s="6">
+        <v>0</v>
+      </c>
+      <c r="Q13" s="3"/>
+      <c r="R13" s="5">
         <v>1142787782</v>
-      </c>
-      <c r="R13" s="5">
-        <v>158723</v>
       </c>
       <c r="S13" s="5">
         <v>158723</v>
       </c>
-      <c r="T13" s="2">
+      <c r="T13" s="5">
+        <v>158723</v>
+      </c>
+      <c r="U13" s="2">
         <v>101.58271999999999</v>
       </c>
-      <c r="U13" s="2">
+      <c r="V13" s="2">
         <v>154.91364799999999</v>
       </c>
-      <c r="V13" s="5">
+      <c r="W13" s="5">
         <v>1737178702</v>
       </c>
-      <c r="W13" s="3"/>
-    </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X13" s="3"/>
+    </row>
+    <row r="14" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A14" s="2">
         <v>7199.2423429999999</v>
       </c>
@@ -1560,31 +1675,35 @@
       <c r="N14" s="5">
         <v>0</v>
       </c>
-      <c r="O14" s="6">
-        <v>0</v>
-      </c>
-      <c r="P14" s="3"/>
-      <c r="Q14" s="5">
+      <c r="O14" s="5">
+        <f>Table1[[#This Row],[Losses '[ratio'](%)]]*1000000</f>
+        <v>0</v>
+      </c>
+      <c r="P14" s="6">
+        <v>0</v>
+      </c>
+      <c r="Q14" s="3"/>
+      <c r="R14" s="5">
         <v>786462075</v>
-      </c>
-      <c r="R14" s="5">
-        <v>109242</v>
       </c>
       <c r="S14" s="5">
         <v>109242</v>
       </c>
-      <c r="T14" s="2">
+      <c r="T14" s="5">
+        <v>109242</v>
+      </c>
+      <c r="U14" s="2">
         <v>69.914879999999997</v>
       </c>
-      <c r="U14" s="2">
+      <c r="V14" s="2">
         <v>106.620192</v>
       </c>
-      <c r="V14" s="5">
+      <c r="W14" s="5">
         <v>2093242725</v>
       </c>
-      <c r="W14" s="3"/>
-    </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X14" s="3"/>
+    </row>
+    <row r="15" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A15" s="2">
         <v>7199.5849619999999</v>
       </c>
@@ -1627,31 +1746,35 @@
       <c r="N15" s="5">
         <v>0</v>
       </c>
-      <c r="O15" s="6">
-        <v>0</v>
-      </c>
-      <c r="P15" s="3"/>
-      <c r="Q15" s="5">
+      <c r="O15" s="5">
+        <f>Table1[[#This Row],[Losses '[ratio'](%)]]*1000000</f>
+        <v>0</v>
+      </c>
+      <c r="P15" s="6">
+        <v>0</v>
+      </c>
+      <c r="Q15" s="3"/>
+      <c r="R15" s="5">
         <v>298640345</v>
-      </c>
-      <c r="R15" s="5">
-        <v>41480</v>
       </c>
       <c r="S15" s="5">
         <v>41480</v>
       </c>
-      <c r="T15" s="2">
+      <c r="T15" s="5">
+        <v>41480</v>
+      </c>
+      <c r="U15" s="2">
         <v>26.5472</v>
       </c>
-      <c r="U15" s="2">
+      <c r="V15" s="2">
         <v>40.484479999999998</v>
       </c>
-      <c r="V15" s="5">
+      <c r="W15" s="5">
         <v>-1713770671</v>
       </c>
-      <c r="W15" s="3"/>
-    </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X15" s="3"/>
+    </row>
+    <row r="16" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A16" s="2">
         <v>7199.5873920000004</v>
       </c>
@@ -1694,31 +1817,35 @@
       <c r="N16" s="5">
         <v>0</v>
       </c>
-      <c r="O16" s="6">
-        <v>0</v>
-      </c>
-      <c r="P16" s="3"/>
-      <c r="Q16" s="5">
+      <c r="O16" s="5">
+        <f>Table1[[#This Row],[Losses '[ratio'](%)]]*1000000</f>
+        <v>0</v>
+      </c>
+      <c r="P16" s="6">
+        <v>0</v>
+      </c>
+      <c r="Q16" s="3"/>
+      <c r="R16" s="5">
         <v>290432265</v>
-      </c>
-      <c r="R16" s="5">
-        <v>40340</v>
       </c>
       <c r="S16" s="5">
         <v>40340</v>
       </c>
-      <c r="T16" s="2">
+      <c r="T16" s="5">
+        <v>40340</v>
+      </c>
+      <c r="U16" s="2">
         <v>25.817599999999999</v>
       </c>
-      <c r="U16" s="2">
+      <c r="V16" s="2">
         <v>39.371839999999999</v>
       </c>
-      <c r="V16" s="5">
+      <c r="W16" s="5">
         <v>-1705561701</v>
       </c>
-      <c r="W16" s="3"/>
-    </row>
-    <row r="17" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X16" s="3"/>
+    </row>
+    <row r="17" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A17" s="2">
         <v>7199.3321910000004</v>
       </c>
@@ -1761,31 +1888,35 @@
       <c r="N17" s="5">
         <v>0</v>
       </c>
-      <c r="O17" s="6">
-        <v>0</v>
-      </c>
-      <c r="P17" s="3"/>
-      <c r="Q17" s="5">
+      <c r="O17" s="5">
+        <f>Table1[[#This Row],[Losses '[ratio'](%)]]*1000000</f>
+        <v>0</v>
+      </c>
+      <c r="P17" s="6">
+        <v>0</v>
+      </c>
+      <c r="Q17" s="3"/>
+      <c r="R17" s="5">
         <v>672940595</v>
-      </c>
-      <c r="R17" s="5">
-        <v>93472</v>
       </c>
       <c r="S17" s="5">
         <v>93472</v>
       </c>
-      <c r="T17" s="2">
+      <c r="T17" s="5">
+        <v>93472</v>
+      </c>
+      <c r="U17" s="2">
         <v>59.82208</v>
       </c>
-      <c r="U17" s="2">
+      <c r="V17" s="2">
         <v>91.228672000000003</v>
       </c>
-      <c r="V17" s="5">
+      <c r="W17" s="5">
         <v>-2088168286</v>
       </c>
-      <c r="W17" s="3"/>
-    </row>
-    <row r="18" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X17" s="3"/>
+    </row>
+    <row r="18" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A18" s="2">
         <v>7199.9253470000003</v>
       </c>
@@ -1828,31 +1959,35 @@
       <c r="N18" s="5">
         <v>0</v>
       </c>
-      <c r="O18" s="6">
-        <v>0</v>
-      </c>
-      <c r="P18" s="3"/>
-      <c r="Q18" s="5">
+      <c r="O18" s="5">
+        <f>Table1[[#This Row],[Losses '[ratio'](%)]]*1000000</f>
+        <v>0</v>
+      </c>
+      <c r="P18" s="6">
+        <v>0</v>
+      </c>
+      <c r="Q18" s="3"/>
+      <c r="R18" s="5">
         <v>297983683</v>
-      </c>
-      <c r="R18" s="5">
-        <v>41387</v>
       </c>
       <c r="S18" s="5">
         <v>41387</v>
       </c>
-      <c r="T18" s="2">
+      <c r="T18" s="5">
+        <v>41387</v>
+      </c>
+      <c r="U18" s="2">
         <v>2946.7543999999998</v>
       </c>
-      <c r="U18" s="2">
+      <c r="V18" s="2">
         <v>2960.6604320000001</v>
       </c>
-      <c r="V18" s="5">
+      <c r="W18" s="5">
         <v>-1712977862</v>
       </c>
-      <c r="W18" s="3"/>
-    </row>
-    <row r="19" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X18" s="3"/>
+    </row>
+    <row r="19" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A19" s="2">
         <v>7199.9606190000004</v>
       </c>
@@ -1895,31 +2030,35 @@
       <c r="N19" s="5">
         <v>0</v>
       </c>
-      <c r="O19" s="6">
-        <v>0</v>
-      </c>
-      <c r="P19" s="3"/>
-      <c r="Q19" s="5">
+      <c r="O19" s="5">
+        <f>Table1[[#This Row],[Losses '[ratio'](%)]]*1000000</f>
+        <v>0</v>
+      </c>
+      <c r="P19" s="6">
+        <v>0</v>
+      </c>
+      <c r="Q19" s="3"/>
+      <c r="R19" s="5">
         <v>748535440</v>
-      </c>
-      <c r="R19" s="5">
-        <v>103963</v>
       </c>
       <c r="S19" s="5">
         <v>103963</v>
       </c>
-      <c r="T19" s="2">
+      <c r="T19" s="5">
+        <v>103963</v>
+      </c>
+      <c r="U19" s="2">
         <v>7402.1656000000003</v>
       </c>
-      <c r="U19" s="2">
+      <c r="V19" s="2">
         <v>7437.0971680000002</v>
       </c>
-      <c r="V19" s="5">
+      <c r="W19" s="5">
         <v>2131456292</v>
       </c>
-      <c r="W19" s="3"/>
-    </row>
-    <row r="20" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X19" s="3"/>
+    </row>
+    <row r="20" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A20" s="2">
         <v>7199.9260370000002</v>
       </c>
@@ -1962,31 +2101,35 @@
       <c r="N20" s="5">
         <v>0</v>
       </c>
-      <c r="O20" s="6">
-        <v>0</v>
-      </c>
-      <c r="P20" s="3"/>
-      <c r="Q20" s="5">
+      <c r="O20" s="5">
+        <f>Table1[[#This Row],[Losses '[ratio'](%)]]*1000000</f>
+        <v>0</v>
+      </c>
+      <c r="P20" s="6">
+        <v>0</v>
+      </c>
+      <c r="Q20" s="3"/>
+      <c r="R20" s="5">
         <v>304289928</v>
-      </c>
-      <c r="R20" s="5">
-        <v>42262</v>
       </c>
       <c r="S20" s="5">
         <v>42262</v>
       </c>
-      <c r="T20" s="2">
+      <c r="T20" s="5">
+        <v>42262</v>
+      </c>
+      <c r="U20" s="2">
         <v>3009.0544</v>
       </c>
-      <c r="U20" s="2">
+      <c r="V20" s="2">
         <v>3023.2544320000002</v>
       </c>
-      <c r="V20" s="5">
+      <c r="W20" s="5">
         <v>-1719283768</v>
       </c>
-      <c r="W20" s="3"/>
-    </row>
-    <row r="21" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X20" s="3"/>
+    </row>
+    <row r="21" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A21" s="2">
         <v>7199.9588000000003</v>
       </c>
@@ -2029,31 +2172,35 @@
       <c r="N21" s="5">
         <v>0</v>
       </c>
-      <c r="O21" s="6">
-        <v>0</v>
-      </c>
-      <c r="P21" s="3"/>
-      <c r="Q21" s="5">
+      <c r="O21" s="5">
+        <f>Table1[[#This Row],[Losses '[ratio'](%)]]*1000000</f>
+        <v>0</v>
+      </c>
+      <c r="P21" s="6">
+        <v>0</v>
+      </c>
+      <c r="Q21" s="3"/>
+      <c r="R21" s="5">
         <v>502496763</v>
-      </c>
-      <c r="R21" s="5">
-        <v>69791</v>
       </c>
       <c r="S21" s="5">
         <v>69791</v>
       </c>
-      <c r="T21" s="2">
+      <c r="T21" s="5">
+        <v>69791</v>
+      </c>
+      <c r="U21" s="2">
         <v>4969.1192000000001</v>
       </c>
-      <c r="U21" s="2">
+      <c r="V21" s="2">
         <v>4992.5689759999996</v>
       </c>
-      <c r="V21" s="5">
+      <c r="W21" s="5">
         <v>-1917475516</v>
       </c>
-      <c r="W21" s="3"/>
-    </row>
-    <row r="22" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X21" s="3"/>
+    </row>
+    <row r="22" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A22" s="2">
         <v>7199.9253179999996</v>
       </c>
@@ -2096,31 +2243,35 @@
       <c r="N22" s="5">
         <v>0</v>
       </c>
-      <c r="O22" s="6">
-        <v>0</v>
-      </c>
-      <c r="P22" s="3"/>
-      <c r="Q22" s="5">
+      <c r="O22" s="5">
+        <f>Table1[[#This Row],[Losses '[ratio'](%)]]*1000000</f>
+        <v>0</v>
+      </c>
+      <c r="P22" s="6">
+        <v>0</v>
+      </c>
+      <c r="Q22" s="3"/>
+      <c r="R22" s="5">
         <v>296045951</v>
-      </c>
-      <c r="R22" s="5">
-        <v>41117</v>
       </c>
       <c r="S22" s="5">
         <v>41117</v>
       </c>
-      <c r="T22" s="2">
+      <c r="T22" s="5">
+        <v>41117</v>
+      </c>
+      <c r="U22" s="2">
         <v>2927.5304000000001</v>
       </c>
-      <c r="U22" s="2">
+      <c r="V22" s="2">
         <v>2941.3457119999998</v>
       </c>
-      <c r="V22" s="5">
+      <c r="W22" s="5">
         <v>-1711040160</v>
       </c>
-      <c r="W22" s="3"/>
-    </row>
-    <row r="23" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X22" s="3"/>
+    </row>
+    <row r="23" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A23" s="2">
         <v>7199.9608870000002</v>
       </c>
@@ -2163,31 +2314,35 @@
       <c r="N23" s="5">
         <v>0</v>
       </c>
-      <c r="O23" s="6">
-        <v>0</v>
-      </c>
-      <c r="P23" s="3"/>
-      <c r="Q23" s="5">
+      <c r="O23" s="5">
+        <f>Table1[[#This Row],[Losses '[ratio'](%)]]*1000000</f>
+        <v>0</v>
+      </c>
+      <c r="P23" s="6">
+        <v>0</v>
+      </c>
+      <c r="Q23" s="3"/>
+      <c r="R23" s="5">
         <v>732560345</v>
-      </c>
-      <c r="R23" s="5">
-        <v>101745</v>
       </c>
       <c r="S23" s="5">
         <v>101745</v>
       </c>
-      <c r="T23" s="2">
+      <c r="T23" s="5">
+        <v>101745</v>
+      </c>
+      <c r="U23" s="2">
         <v>7244.2439999999997</v>
       </c>
-      <c r="U23" s="2">
+      <c r="V23" s="2">
         <v>7278.4303200000004</v>
       </c>
-      <c r="V23" s="5">
+      <c r="W23" s="5">
         <v>2147431334</v>
       </c>
-      <c r="W23" s="3"/>
-    </row>
-    <row r="24" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X23" s="3"/>
+    </row>
+    <row r="24" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A24" s="2">
         <v>7199.9259529999999</v>
       </c>
@@ -2230,31 +2385,35 @@
       <c r="N24" s="5">
         <v>0</v>
       </c>
-      <c r="O24" s="6">
-        <v>0</v>
-      </c>
-      <c r="P24" s="3"/>
-      <c r="Q24" s="5">
+      <c r="O24" s="5">
+        <f>Table1[[#This Row],[Losses '[ratio'](%)]]*1000000</f>
+        <v>0</v>
+      </c>
+      <c r="P24" s="6">
+        <v>0</v>
+      </c>
+      <c r="Q24" s="3"/>
+      <c r="R24" s="5">
         <v>301738842</v>
-      </c>
-      <c r="R24" s="5">
-        <v>41908</v>
       </c>
       <c r="S24" s="5">
         <v>41908</v>
       </c>
-      <c r="T24" s="2">
+      <c r="T24" s="5">
+        <v>41908</v>
+      </c>
+      <c r="U24" s="2">
         <v>2983.8496</v>
       </c>
-      <c r="U24" s="2">
+      <c r="V24" s="2">
         <v>2997.9306879999999</v>
       </c>
-      <c r="V24" s="5">
+      <c r="W24" s="5">
         <v>-1716732740</v>
       </c>
-      <c r="W24" s="3"/>
-    </row>
-    <row r="25" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X24" s="3"/>
+    </row>
+    <row r="25" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A25" s="2">
         <v>7199.9577639999998</v>
       </c>
@@ -2297,31 +2456,35 @@
       <c r="N25" s="5">
         <v>0</v>
       </c>
-      <c r="O25" s="6">
-        <v>0</v>
-      </c>
-      <c r="P25" s="3"/>
-      <c r="Q25" s="5">
+      <c r="O25" s="5">
+        <f>Table1[[#This Row],[Losses '[ratio'](%)]]*1000000</f>
+        <v>0</v>
+      </c>
+      <c r="P25" s="6">
+        <v>0</v>
+      </c>
+      <c r="Q25" s="3"/>
+      <c r="R25" s="5">
         <v>685587575</v>
-      </c>
-      <c r="R25" s="5">
-        <v>95221</v>
       </c>
       <c r="S25" s="5">
         <v>95221</v>
       </c>
-      <c r="T25" s="2">
+      <c r="T25" s="5">
+        <v>95221</v>
+      </c>
+      <c r="U25" s="2">
         <v>6779.7352000000001</v>
       </c>
-      <c r="U25" s="2">
+      <c r="V25" s="2">
         <v>6811.729456</v>
       </c>
-      <c r="V25" s="5">
+      <c r="W25" s="5">
         <v>-2100564911</v>
       </c>
-      <c r="W25" s="3"/>
-    </row>
-    <row r="26" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X25" s="3"/>
+    </row>
+    <row r="26" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A26" s="2">
         <v>7199.9112759999998</v>
       </c>
@@ -2364,31 +2527,35 @@
       <c r="N26" s="5">
         <v>0</v>
       </c>
-      <c r="O26" s="6">
-        <v>0</v>
-      </c>
-      <c r="P26" s="3"/>
-      <c r="Q26" s="5">
+      <c r="O26" s="5">
+        <f>Table1[[#This Row],[Losses '[ratio'](%)]]*1000000</f>
+        <v>0</v>
+      </c>
+      <c r="P26" s="6">
+        <v>0</v>
+      </c>
+      <c r="Q26" s="3"/>
+      <c r="R26" s="5">
         <v>299659524</v>
-      </c>
-      <c r="R26" s="5">
-        <v>41619</v>
       </c>
       <c r="S26" s="5">
         <v>41619</v>
       </c>
-      <c r="T26" s="2">
+      <c r="T26" s="5">
+        <v>41619</v>
+      </c>
+      <c r="U26" s="2">
         <v>2963.2728000000002</v>
       </c>
-      <c r="U26" s="2">
+      <c r="V26" s="2">
         <v>2977.2567840000002</v>
       </c>
-      <c r="V26" s="5">
+      <c r="W26" s="5">
         <v>-1714659314</v>
       </c>
-      <c r="W26" s="3"/>
-    </row>
-    <row r="27" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X26" s="3"/>
+    </row>
+    <row r="27" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A27" s="2">
         <v>7199.961585</v>
       </c>
@@ -2431,31 +2598,35 @@
       <c r="N27" s="5">
         <v>0</v>
       </c>
-      <c r="O27" s="6">
-        <v>0</v>
-      </c>
-      <c r="P27" s="3"/>
-      <c r="Q27" s="5">
+      <c r="O27" s="5">
+        <f>Table1[[#This Row],[Losses '[ratio'](%)]]*1000000</f>
+        <v>0</v>
+      </c>
+      <c r="P27" s="6">
+        <v>0</v>
+      </c>
+      <c r="Q27" s="3"/>
+      <c r="R27" s="5">
         <v>770890864</v>
-      </c>
-      <c r="R27" s="5">
-        <v>107068</v>
       </c>
       <c r="S27" s="5">
         <v>107068</v>
       </c>
-      <c r="T27" s="2">
+      <c r="T27" s="5">
+        <v>107068</v>
+      </c>
+      <c r="U27" s="2">
         <v>7623.2416000000003</v>
       </c>
-      <c r="U27" s="2">
+      <c r="V27" s="2">
         <v>7659.2164480000001</v>
       </c>
-      <c r="V27" s="5">
+      <c r="W27" s="5">
         <v>2109101477</v>
       </c>
-      <c r="W27" s="3"/>
-    </row>
-    <row r="28" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X27" s="3"/>
+    </row>
+    <row r="28" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A28" s="2">
         <v>7199.960247</v>
       </c>
@@ -2498,31 +2669,35 @@
       <c r="N28" s="5">
         <v>0</v>
       </c>
-      <c r="O28" s="6">
-        <v>0</v>
-      </c>
-      <c r="P28" s="3"/>
-      <c r="Q28" s="5">
+      <c r="O28" s="5">
+        <f>Table1[[#This Row],[Losses '[ratio'](%)]]*1000000</f>
+        <v>0</v>
+      </c>
+      <c r="P28" s="6">
+        <v>0</v>
+      </c>
+      <c r="Q28" s="3"/>
+      <c r="R28" s="5">
         <v>631967749</v>
-      </c>
-      <c r="R28" s="5">
-        <v>87773</v>
       </c>
       <c r="S28" s="5">
         <v>87773</v>
       </c>
-      <c r="T28" s="2">
+      <c r="T28" s="5">
+        <v>87773</v>
+      </c>
+      <c r="U28" s="2">
         <v>6249.4376000000002</v>
       </c>
-      <c r="U28" s="2">
+      <c r="V28" s="2">
         <v>6278.9293280000002</v>
       </c>
-      <c r="V28" s="5">
+      <c r="W28" s="5">
         <v>-2046944628</v>
       </c>
-      <c r="W28" s="3"/>
-    </row>
-    <row r="29" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X28" s="3"/>
+    </row>
+    <row r="29" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A29" s="2">
         <v>7199.9253040000003</v>
       </c>
@@ -2565,31 +2740,35 @@
       <c r="N29" s="5">
         <v>0</v>
       </c>
-      <c r="O29" s="6">
-        <v>0</v>
-      </c>
-      <c r="P29" s="3"/>
-      <c r="Q29" s="5">
+      <c r="O29" s="5">
+        <f>Table1[[#This Row],[Losses '[ratio'](%)]]*1000000</f>
+        <v>0</v>
+      </c>
+      <c r="P29" s="6">
+        <v>0</v>
+      </c>
+      <c r="Q29" s="3"/>
+      <c r="R29" s="5">
         <v>295439032</v>
-      </c>
-      <c r="R29" s="5">
-        <v>41033</v>
       </c>
       <c r="S29" s="5">
         <v>41033</v>
       </c>
-      <c r="T29" s="2">
+      <c r="T29" s="5">
+        <v>41033</v>
+      </c>
+      <c r="U29" s="2">
         <v>2921.5495999999998</v>
       </c>
-      <c r="U29" s="2">
+      <c r="V29" s="2">
         <v>2935.3366879999999</v>
       </c>
-      <c r="V29" s="5">
+      <c r="W29" s="5">
         <v>-1710433253</v>
       </c>
-      <c r="W29" s="3"/>
-    </row>
-    <row r="30" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X29" s="3"/>
+    </row>
+    <row r="30" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A30" s="2">
         <v>7199.9259629999997</v>
       </c>
@@ -2632,31 +2811,35 @@
       <c r="N30" s="5">
         <v>0</v>
       </c>
-      <c r="O30" s="6">
-        <v>0</v>
-      </c>
-      <c r="P30" s="3"/>
-      <c r="Q30" s="5">
+      <c r="O30" s="5">
+        <f>Table1[[#This Row],[Losses '[ratio'](%)]]*1000000</f>
+        <v>0</v>
+      </c>
+      <c r="P30" s="6">
+        <v>0</v>
+      </c>
+      <c r="Q30" s="3"/>
+      <c r="R30" s="5">
         <v>297062009</v>
-      </c>
-      <c r="R30" s="5">
-        <v>41259</v>
       </c>
       <c r="S30" s="5">
         <v>41259</v>
       </c>
-      <c r="T30" s="2">
+      <c r="T30" s="5">
+        <v>41259</v>
+      </c>
+      <c r="U30" s="2">
         <v>2937.6408000000001</v>
       </c>
-      <c r="U30" s="2">
+      <c r="V30" s="2">
         <v>2951.5038239999999</v>
       </c>
-      <c r="V30" s="5">
+      <c r="W30" s="5">
         <v>-1712055951</v>
       </c>
-      <c r="W30" s="3"/>
-    </row>
-    <row r="31" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X30" s="3"/>
+    </row>
+    <row r="31" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A31" s="2">
         <v>7199.9253429999999</v>
       </c>
@@ -2699,31 +2882,35 @@
       <c r="N31" s="5">
         <v>0</v>
       </c>
-      <c r="O31" s="6">
-        <v>0</v>
-      </c>
-      <c r="P31" s="3"/>
-      <c r="Q31" s="5">
+      <c r="O31" s="5">
+        <f>Table1[[#This Row],[Losses '[ratio'](%)]]*1000000</f>
+        <v>0</v>
+      </c>
+      <c r="P31" s="6">
+        <v>0</v>
+      </c>
+      <c r="Q31" s="3"/>
+      <c r="R31" s="5">
         <v>296775187</v>
-      </c>
-      <c r="R31" s="5">
-        <v>41219</v>
       </c>
       <c r="S31" s="5">
         <v>41219</v>
       </c>
-      <c r="T31" s="2">
+      <c r="T31" s="5">
+        <v>41219</v>
+      </c>
+      <c r="U31" s="2">
         <v>2934.7928000000002</v>
       </c>
-      <c r="U31" s="2">
+      <c r="V31" s="2">
         <v>2948.6423840000002</v>
       </c>
-      <c r="V31" s="5">
+      <c r="W31" s="5">
         <v>-1711769380</v>
       </c>
-      <c r="W31" s="3"/>
-    </row>
-    <row r="32" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X31" s="3"/>
+    </row>
+    <row r="32" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A32" s="2">
         <v>7199.9594370000004</v>
       </c>
@@ -2766,98 +2953,106 @@
       <c r="N32" s="5">
         <v>0</v>
       </c>
-      <c r="O32" s="6">
-        <v>0</v>
-      </c>
-      <c r="P32" s="3"/>
-      <c r="Q32" s="5">
+      <c r="O32" s="5">
+        <f>Table1[[#This Row],[Losses '[ratio'](%)]]*1000000</f>
+        <v>0</v>
+      </c>
+      <c r="P32" s="6">
+        <v>0</v>
+      </c>
+      <c r="Q32" s="3"/>
+      <c r="R32" s="5">
         <v>636385309</v>
-      </c>
-      <c r="R32" s="5">
-        <v>88387</v>
       </c>
       <c r="S32" s="5">
         <v>88387</v>
       </c>
-      <c r="T32" s="2">
+      <c r="T32" s="5">
+        <v>88387</v>
+      </c>
+      <c r="U32" s="2">
         <v>6293.1544000000004</v>
       </c>
-      <c r="U32" s="2">
+      <c r="V32" s="2">
         <v>6322.8524319999997</v>
       </c>
-      <c r="V32" s="5">
+      <c r="W32" s="5">
         <v>-2051362468</v>
       </c>
-      <c r="W32" s="3"/>
-    </row>
-    <row r="33" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A33" s="2">
+      <c r="X32" s="3"/>
+    </row>
+    <row r="33" spans="1:24" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="7">
         <v>7199.973798</v>
       </c>
-      <c r="B33" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="C33" s="4" t="s">
+      <c r="B33" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C33" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="D33" s="3" t="s">
+      <c r="D33" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="E33" s="3" t="s">
+      <c r="E33" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="F33" s="3">
+      <c r="F33" s="8">
         <v>8110</v>
       </c>
-      <c r="G33" s="5">
-        <v>2500</v>
-      </c>
-      <c r="H33" s="5">
+      <c r="G33" s="10">
+        <v>2500</v>
+      </c>
+      <c r="H33" s="10">
         <v>65000</v>
       </c>
-      <c r="I33" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="J33" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="K33" s="3">
-        <v>0</v>
-      </c>
-      <c r="L33" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="M33" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="N33" s="5">
-        <v>0</v>
-      </c>
-      <c r="O33" s="6">
-        <v>0</v>
-      </c>
-      <c r="P33" s="3"/>
-      <c r="Q33" s="5">
+      <c r="I33" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="J33" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="K33" s="8">
+        <v>0</v>
+      </c>
+      <c r="L33" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="M33" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="N33" s="10">
+        <v>0</v>
+      </c>
+      <c r="O33" s="10">
+        <f>Table1[[#This Row],[Losses '[ratio'](%)]]*1000000</f>
+        <v>0</v>
+      </c>
+      <c r="P33" s="11">
+        <v>0</v>
+      </c>
+      <c r="Q33" s="8"/>
+      <c r="R33" s="10">
         <v>113776812</v>
       </c>
-      <c r="R33" s="5">
+      <c r="S33" s="10">
         <v>15802</v>
       </c>
-      <c r="S33" s="5">
+      <c r="T33" s="10">
         <v>126416</v>
       </c>
-      <c r="T33" s="2">
+      <c r="U33" s="7">
         <v>8217.0400000000009</v>
       </c>
-      <c r="U33" s="2">
+      <c r="V33" s="7">
         <v>8252.4364800000003</v>
       </c>
-      <c r="V33" s="5">
+      <c r="W33" s="10">
         <v>-1528753453</v>
       </c>
-      <c r="W33" s="3"/>
-    </row>
-    <row r="34" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X33" s="8"/>
+    </row>
+    <row r="34" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A34" s="2">
         <v>7199.9664439999997</v>
       </c>
@@ -2900,100 +3095,108 @@
       <c r="N34" s="5">
         <v>11</v>
       </c>
-      <c r="O34" s="6">
+      <c r="O34" s="5">
+        <f>Table1[[#This Row],[Losses '[ratio'](%)]]*1000000</f>
+        <v>9.0940239068330167E-2</v>
+      </c>
+      <c r="P34" s="6">
         <v>9.0940239068330173E-8</v>
       </c>
-      <c r="P34" s="3" t="s">
+      <c r="Q34" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="Q34" s="5">
+      <c r="R34" s="5">
         <v>120958556</v>
       </c>
-      <c r="R34" s="5">
+      <c r="S34" s="5">
         <v>16799</v>
       </c>
-      <c r="S34" s="5">
+      <c r="T34" s="5">
         <v>134392</v>
       </c>
-      <c r="T34" s="2">
+      <c r="U34" s="2">
         <v>8735.48</v>
       </c>
-      <c r="U34" s="2">
+      <c r="V34" s="2">
         <v>8773.1097599999994</v>
       </c>
-      <c r="V34" s="5">
+      <c r="W34" s="5">
         <v>-1535938066</v>
       </c>
-      <c r="W34" s="3"/>
-    </row>
-    <row r="35" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A35" s="2">
+      <c r="X34" s="3"/>
+    </row>
+    <row r="35" spans="1:24" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="7">
         <v>7199.9726449999998</v>
       </c>
-      <c r="B35" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="C35" s="4" t="s">
+      <c r="B35" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C35" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="D35" s="3" t="s">
+      <c r="D35" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="E35" s="3" t="s">
+      <c r="E35" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="F35" s="3">
+      <c r="F35" s="8">
         <v>8410</v>
       </c>
-      <c r="G35" s="5">
-        <v>2500</v>
-      </c>
-      <c r="H35" s="5">
+      <c r="G35" s="10">
+        <v>2500</v>
+      </c>
+      <c r="H35" s="10">
         <v>65000</v>
       </c>
-      <c r="I35" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="J35" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="K35" s="3">
-        <v>0</v>
-      </c>
-      <c r="L35" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="M35" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="N35" s="5">
-        <v>0</v>
-      </c>
-      <c r="O35" s="6">
-        <v>0</v>
-      </c>
-      <c r="P35" s="3"/>
-      <c r="Q35" s="5">
+      <c r="I35" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="J35" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="K35" s="8">
+        <v>0</v>
+      </c>
+      <c r="L35" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="M35" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="N35" s="10">
+        <v>0</v>
+      </c>
+      <c r="O35" s="10">
+        <f>Table1[[#This Row],[Losses '[ratio'](%)]]*1000000</f>
+        <v>0</v>
+      </c>
+      <c r="P35" s="11">
+        <v>0</v>
+      </c>
+      <c r="Q35" s="8"/>
+      <c r="R35" s="10">
         <v>113482864</v>
       </c>
-      <c r="R35" s="5">
+      <c r="S35" s="10">
         <v>15761</v>
       </c>
-      <c r="S35" s="5">
+      <c r="T35" s="10">
         <v>126088</v>
       </c>
-      <c r="T35" s="2">
+      <c r="U35" s="7">
         <v>8195.7199999999993</v>
       </c>
-      <c r="U35" s="2">
+      <c r="V35" s="7">
         <v>8231.0246399999996</v>
       </c>
-      <c r="V35" s="5">
+      <c r="W35" s="10">
         <v>-1528459969</v>
       </c>
-      <c r="W35" s="3"/>
-    </row>
-    <row r="36" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X35" s="8"/>
+    </row>
+    <row r="36" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A36" s="2">
         <v>7199.9632300000003</v>
       </c>
@@ -3036,33 +3239,37 @@
       <c r="N36" s="5">
         <v>8</v>
       </c>
-      <c r="O36" s="6">
+      <c r="O36" s="5">
+        <f>Table1[[#This Row],[Losses '[ratio'](%)]]*1000000</f>
+        <v>5.8198369374807518E-2</v>
+      </c>
+      <c r="P36" s="6">
         <v>5.8198369374807518E-8</v>
       </c>
-      <c r="P36" s="3" t="s">
+      <c r="Q36" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="Q36" s="5">
+      <c r="R36" s="5">
         <v>137460896</v>
       </c>
-      <c r="R36" s="5">
+      <c r="S36" s="5">
         <v>19091</v>
       </c>
-      <c r="S36" s="5">
+      <c r="T36" s="5">
         <v>152728</v>
       </c>
-      <c r="T36" s="2">
+      <c r="U36" s="2">
         <v>9927.32</v>
       </c>
-      <c r="U36" s="2">
+      <c r="V36" s="2">
         <v>9970.0838399999993</v>
       </c>
-      <c r="V36" s="5">
+      <c r="W36" s="5">
         <v>-1552441527</v>
       </c>
-      <c r="W36" s="3"/>
-    </row>
-    <row r="37" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X36" s="3"/>
+    </row>
+    <row r="37" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A37" s="2">
         <v>7199.9644349999999</v>
       </c>
@@ -3105,167 +3312,179 @@
       <c r="N37" s="5">
         <v>9</v>
       </c>
-      <c r="O37" s="6">
+      <c r="O37" s="5">
+        <f>Table1[[#This Row],[Losses '[ratio'](%)]]*1000000</f>
+        <v>7.8194112871238383E-2</v>
+      </c>
+      <c r="P37" s="6">
         <v>7.8194112871238384E-8</v>
       </c>
-      <c r="P37" s="3" t="s">
+      <c r="Q37" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="Q37" s="5">
+      <c r="R37" s="5">
         <v>115098179</v>
       </c>
-      <c r="R37" s="5">
+      <c r="S37" s="5">
         <v>15985</v>
       </c>
-      <c r="S37" s="5">
+      <c r="T37" s="5">
         <v>127880</v>
       </c>
-      <c r="T37" s="2">
+      <c r="U37" s="2">
         <v>8312.2000000000007</v>
       </c>
-      <c r="U37" s="2">
+      <c r="V37" s="2">
         <v>8348.0064000000002</v>
       </c>
-      <c r="V37" s="5">
+      <c r="W37" s="5">
         <v>-1530078552</v>
       </c>
-      <c r="W37" s="3"/>
-    </row>
-    <row r="38" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A38" s="2">
+      <c r="X37" s="3"/>
+    </row>
+    <row r="38" spans="1:24" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="7">
         <v>7199.9705809999996</v>
       </c>
-      <c r="B38" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="C38" s="4" t="s">
+      <c r="B38" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C38" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="D38" s="3" t="s">
+      <c r="D38" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="E38" s="3" t="s">
+      <c r="E38" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="F38" s="3">
+      <c r="F38" s="8">
         <v>8100</v>
       </c>
-      <c r="G38" s="5">
-        <v>2500</v>
-      </c>
-      <c r="H38" s="5">
+      <c r="G38" s="10">
+        <v>2500</v>
+      </c>
+      <c r="H38" s="10">
         <v>65000</v>
       </c>
-      <c r="I38" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="J38" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="K38" s="3">
-        <v>0</v>
-      </c>
-      <c r="L38" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="M38" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="N38" s="5">
-        <v>0</v>
-      </c>
-      <c r="O38" s="6">
-        <v>0</v>
-      </c>
-      <c r="P38" s="3"/>
-      <c r="Q38" s="5">
+      <c r="I38" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="J38" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="K38" s="8">
+        <v>0</v>
+      </c>
+      <c r="L38" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="M38" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="N38" s="10">
+        <v>0</v>
+      </c>
+      <c r="O38" s="10">
+        <f>Table1[[#This Row],[Losses '[ratio'](%)]]*1000000</f>
+        <v>0</v>
+      </c>
+      <c r="P38" s="11">
+        <v>0</v>
+      </c>
+      <c r="Q38" s="8"/>
+      <c r="R38" s="10">
         <v>113077353</v>
       </c>
-      <c r="R38" s="5">
+      <c r="S38" s="10">
         <v>15705</v>
       </c>
-      <c r="S38" s="5">
+      <c r="T38" s="10">
         <v>125640</v>
       </c>
-      <c r="T38" s="2">
+      <c r="U38" s="7">
         <v>8166.6</v>
       </c>
-      <c r="U38" s="2">
+      <c r="V38" s="7">
         <v>8201.7792000000009</v>
       </c>
-      <c r="V38" s="5">
+      <c r="W38" s="10">
         <v>-1528055287</v>
       </c>
-      <c r="W38" s="3"/>
-    </row>
-    <row r="39" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A39" s="2">
+      <c r="X38" s="8"/>
+    </row>
+    <row r="39" spans="1:24" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A39" s="7">
         <v>7199.9734680000001</v>
       </c>
-      <c r="B39" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="C39" s="4" t="s">
+      <c r="B39" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C39" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="D39" s="3" t="s">
+      <c r="D39" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="E39" s="3" t="s">
+      <c r="E39" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="F39" s="3">
+      <c r="F39" s="8">
         <v>8400</v>
       </c>
-      <c r="G39" s="5">
-        <v>2500</v>
-      </c>
-      <c r="H39" s="5">
+      <c r="G39" s="10">
+        <v>2500</v>
+      </c>
+      <c r="H39" s="10">
         <v>65000</v>
       </c>
-      <c r="I39" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="J39" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="K39" s="3">
-        <v>0</v>
-      </c>
-      <c r="L39" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="M39" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="N39" s="5">
-        <v>0</v>
-      </c>
-      <c r="O39" s="6">
-        <v>0</v>
-      </c>
-      <c r="P39" s="3"/>
-      <c r="Q39" s="5">
+      <c r="I39" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="J39" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="K39" s="8">
+        <v>0</v>
+      </c>
+      <c r="L39" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="M39" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="N39" s="10">
+        <v>0</v>
+      </c>
+      <c r="O39" s="10">
+        <f>Table1[[#This Row],[Losses '[ratio'](%)]]*1000000</f>
+        <v>0</v>
+      </c>
+      <c r="P39" s="11">
+        <v>0</v>
+      </c>
+      <c r="Q39" s="8"/>
+      <c r="R39" s="10">
         <v>113427792</v>
       </c>
-      <c r="R39" s="5">
+      <c r="S39" s="10">
         <v>15753</v>
       </c>
-      <c r="S39" s="5">
+      <c r="T39" s="10">
         <v>126024</v>
       </c>
-      <c r="T39" s="2">
+      <c r="U39" s="7">
         <v>8191.56</v>
       </c>
-      <c r="U39" s="2">
+      <c r="V39" s="7">
         <v>8226.8467199999996</v>
       </c>
-      <c r="V39" s="5">
+      <c r="W39" s="10">
         <v>-1528404567</v>
       </c>
-      <c r="W39" s="3"/>
-    </row>
-    <row r="40" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X39" s="8"/>
+    </row>
+    <row r="40" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A40" s="2">
         <v>7199.964234</v>
       </c>
@@ -3308,33 +3527,37 @@
       <c r="N40" s="5">
         <v>9</v>
       </c>
-      <c r="O40" s="6">
+      <c r="O40" s="5">
+        <f>Table1[[#This Row],[Losses '[ratio'](%)]]*1000000</f>
+        <v>7.907230057511129E-2</v>
+      </c>
+      <c r="P40" s="6">
         <v>7.9072300575111295E-8</v>
       </c>
-      <c r="P40" s="3" t="s">
+      <c r="Q40" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="Q40" s="5">
+      <c r="R40" s="5">
         <v>113819883</v>
       </c>
-      <c r="R40" s="5">
+      <c r="S40" s="5">
         <v>15808</v>
       </c>
-      <c r="S40" s="5">
+      <c r="T40" s="5">
         <v>126464</v>
       </c>
-      <c r="T40" s="2">
+      <c r="U40" s="2">
         <v>8220.16</v>
       </c>
-      <c r="U40" s="2">
+      <c r="V40" s="2">
         <v>8255.5699199999999</v>
       </c>
-      <c r="V40" s="5">
+      <c r="W40" s="5">
         <v>-1528800348</v>
       </c>
-      <c r="W40" s="3"/>
-    </row>
-    <row r="41" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X40" s="3"/>
+    </row>
+    <row r="41" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A41" s="2">
         <v>7199.9644360000002</v>
       </c>
@@ -3377,102 +3600,110 @@
       <c r="N41" s="5">
         <v>8</v>
       </c>
-      <c r="O41" s="6">
+      <c r="O41" s="5">
+        <f>Table1[[#This Row],[Losses '[ratio'](%)]]*1000000</f>
+        <v>5.819834439532303E-2</v>
+      </c>
+      <c r="P41" s="6">
         <v>5.8198344395323028E-8</v>
       </c>
-      <c r="P41" s="3" t="s">
+      <c r="Q41" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="Q41" s="5">
+      <c r="R41" s="5">
         <v>137460955</v>
       </c>
-      <c r="R41" s="5">
+      <c r="S41" s="5">
         <v>19091</v>
       </c>
-      <c r="S41" s="5">
+      <c r="T41" s="5">
         <v>152728</v>
       </c>
-      <c r="T41" s="2">
+      <c r="U41" s="2">
         <v>9927.32</v>
       </c>
-      <c r="U41" s="2">
+      <c r="V41" s="2">
         <v>9970.0838399999993</v>
       </c>
-      <c r="V41" s="5">
+      <c r="W41" s="5">
         <v>-1552441103</v>
       </c>
-      <c r="W41" s="3"/>
-    </row>
-    <row r="42" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A42" s="2">
+      <c r="X41" s="3"/>
+    </row>
+    <row r="42" spans="1:24" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A42" s="7">
         <v>7199.970311</v>
       </c>
-      <c r="B42" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="C42" s="4" t="s">
+      <c r="B42" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C42" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="D42" s="3" t="s">
+      <c r="D42" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="E42" s="3" t="s">
+      <c r="E42" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="F42" s="3">
+      <c r="F42" s="8">
         <v>8300</v>
       </c>
-      <c r="G42" s="5">
-        <v>2500</v>
-      </c>
-      <c r="H42" s="5">
+      <c r="G42" s="10">
+        <v>2500</v>
+      </c>
+      <c r="H42" s="10">
         <v>65000</v>
       </c>
-      <c r="I42" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="J42" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="K42" s="3">
-        <v>0</v>
-      </c>
-      <c r="L42" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="M42" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="N42" s="5">
+      <c r="I42" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="J42" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="K42" s="8">
+        <v>0</v>
+      </c>
+      <c r="L42" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="M42" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="N42" s="10">
         <v>4313</v>
       </c>
-      <c r="O42" s="6">
+      <c r="O42" s="10">
+        <f>Table1[[#This Row],[Losses '[ratio'](%)]]*1000000</f>
+        <v>39.125602209285681</v>
+      </c>
+      <c r="P42" s="11">
         <v>3.9125602209285682E-5</v>
       </c>
-      <c r="P42" s="3" t="s">
+      <c r="Q42" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="Q42" s="5">
+      <c r="R42" s="10">
         <v>110234725</v>
       </c>
-      <c r="R42" s="5">
+      <c r="S42" s="10">
         <v>15310</v>
       </c>
-      <c r="S42" s="5">
+      <c r="T42" s="10">
         <v>122480</v>
       </c>
-      <c r="T42" s="2">
+      <c r="U42" s="7">
         <v>7961.2</v>
       </c>
-      <c r="U42" s="2">
+      <c r="V42" s="7">
         <v>7995.4943999999996</v>
       </c>
-      <c r="V42" s="5">
+      <c r="W42" s="10">
         <v>-1525212795</v>
       </c>
-      <c r="W42" s="3"/>
-    </row>
-    <row r="43" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X42" s="8"/>
+    </row>
+    <row r="43" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A43" s="2">
         <v>7199.965056</v>
       </c>
@@ -3515,236 +3746,252 @@
       <c r="N43" s="5">
         <v>7</v>
       </c>
-      <c r="O43" s="6">
+      <c r="O43" s="5">
+        <f>Table1[[#This Row],[Losses '[ratio'](%)]]*1000000</f>
+        <v>5.0925191788091663E-2</v>
+      </c>
+      <c r="P43" s="6">
         <v>5.0925191788091662E-8</v>
       </c>
-      <c r="P43" s="3" t="s">
+      <c r="Q43" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="Q43" s="5">
+      <c r="R43" s="5">
         <v>137456527</v>
       </c>
-      <c r="R43" s="5">
+      <c r="S43" s="5">
         <v>19091</v>
       </c>
-      <c r="S43" s="5">
+      <c r="T43" s="5">
         <v>152728</v>
       </c>
-      <c r="T43" s="2">
+      <c r="U43" s="2">
         <v>9927.32</v>
       </c>
-      <c r="U43" s="2">
+      <c r="V43" s="2">
         <v>9970.0838399999993</v>
       </c>
-      <c r="V43" s="5">
+      <c r="W43" s="5">
         <v>-1552436427</v>
       </c>
-      <c r="W43" s="3"/>
-    </row>
-    <row r="44" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A44" s="2">
+      <c r="X43" s="3"/>
+    </row>
+    <row r="44" spans="1:24" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A44" s="7">
         <v>7199.9705309999999</v>
       </c>
-      <c r="B44" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="C44" s="4" t="s">
+      <c r="B44" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C44" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="D44" s="3" t="s">
+      <c r="D44" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="E44" s="3" t="s">
+      <c r="E44" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="F44" s="3">
+      <c r="F44" s="8">
         <v>8200</v>
       </c>
-      <c r="G44" s="5">
-        <v>2500</v>
-      </c>
-      <c r="H44" s="5">
+      <c r="G44" s="10">
+        <v>2500</v>
+      </c>
+      <c r="H44" s="10">
         <v>65000</v>
       </c>
-      <c r="I44" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="J44" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="K44" s="3">
-        <v>0</v>
-      </c>
-      <c r="L44" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="M44" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="N44" s="5">
-        <v>0</v>
-      </c>
-      <c r="O44" s="6">
-        <v>0</v>
-      </c>
-      <c r="P44" s="3"/>
-      <c r="Q44" s="5">
+      <c r="I44" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="J44" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="K44" s="8">
+        <v>0</v>
+      </c>
+      <c r="L44" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="M44" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="N44" s="10">
+        <v>0</v>
+      </c>
+      <c r="O44" s="10">
+        <f>Table1[[#This Row],[Losses '[ratio'](%)]]*1000000</f>
+        <v>0</v>
+      </c>
+      <c r="P44" s="11">
+        <v>0</v>
+      </c>
+      <c r="Q44" s="8"/>
+      <c r="R44" s="10">
         <v>113018436</v>
       </c>
-      <c r="R44" s="5">
+      <c r="S44" s="10">
         <v>15697</v>
       </c>
-      <c r="S44" s="5">
+      <c r="T44" s="10">
         <v>125576</v>
       </c>
-      <c r="T44" s="2">
+      <c r="U44" s="7">
         <v>8162.44</v>
       </c>
-      <c r="U44" s="2">
+      <c r="V44" s="7">
         <v>8197.6012800000008</v>
       </c>
-      <c r="V44" s="5">
+      <c r="W44" s="10">
         <v>-1527996390</v>
       </c>
-      <c r="W44" s="3"/>
-    </row>
-    <row r="45" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A45" s="2">
+      <c r="X44" s="8"/>
+    </row>
+    <row r="45" spans="1:24" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A45" s="7">
         <v>7199.9726259999998</v>
       </c>
-      <c r="B45" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="C45" s="4" t="s">
+      <c r="B45" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C45" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="D45" s="3" t="s">
+      <c r="D45" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="E45" s="3" t="s">
+      <c r="E45" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="F45" s="3">
+      <c r="F45" s="8">
         <v>8310</v>
       </c>
-      <c r="G45" s="5">
-        <v>2500</v>
-      </c>
-      <c r="H45" s="5">
+      <c r="G45" s="10">
+        <v>2500</v>
+      </c>
+      <c r="H45" s="10">
         <v>65000</v>
       </c>
-      <c r="I45" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="J45" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="K45" s="3">
-        <v>0</v>
-      </c>
-      <c r="L45" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="M45" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="N45" s="5">
+      <c r="I45" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="J45" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="K45" s="8">
+        <v>0</v>
+      </c>
+      <c r="L45" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="M45" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="N45" s="10">
         <v>4285</v>
       </c>
-      <c r="O45" s="6">
+      <c r="O45" s="10">
+        <f>Table1[[#This Row],[Losses '[ratio'](%)]]*1000000</f>
+        <v>38.815657034891267</v>
+      </c>
+      <c r="P45" s="11">
         <v>3.8815657034891263E-5</v>
       </c>
-      <c r="P45" s="3" t="s">
+      <c r="Q45" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="Q45" s="5">
+      <c r="R45" s="10">
         <v>110393597</v>
       </c>
-      <c r="R45" s="5">
+      <c r="S45" s="10">
         <v>15332</v>
       </c>
-      <c r="S45" s="5">
+      <c r="T45" s="10">
         <v>122656</v>
       </c>
-      <c r="T45" s="2">
+      <c r="U45" s="7">
         <v>7972.64</v>
       </c>
-      <c r="U45" s="2">
+      <c r="V45" s="7">
         <v>8006.9836800000003</v>
       </c>
-      <c r="V45" s="5">
+      <c r="W45" s="10">
         <v>-1525370740</v>
       </c>
-      <c r="W45" s="3"/>
-    </row>
-    <row r="46" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A46" s="2">
+      <c r="X45" s="8"/>
+    </row>
+    <row r="46" spans="1:24" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A46" s="7">
         <v>7199.9702900000002</v>
       </c>
-      <c r="B46" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="C46" s="4" t="s">
+      <c r="B46" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C46" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="D46" s="3" t="s">
+      <c r="D46" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="E46" s="3" t="s">
+      <c r="E46" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="F46" s="3">
+      <c r="F46" s="8">
         <v>8210</v>
       </c>
-      <c r="G46" s="5">
-        <v>2500</v>
-      </c>
-      <c r="H46" s="5">
+      <c r="G46" s="10">
+        <v>2500</v>
+      </c>
+      <c r="H46" s="10">
         <v>65000</v>
       </c>
-      <c r="I46" s="3" t="b">
-        <v>0</v>
-      </c>
-      <c r="J46" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="K46" s="3">
-        <v>0</v>
-      </c>
-      <c r="L46" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="M46" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="N46" s="5">
-        <v>0</v>
-      </c>
-      <c r="O46" s="6">
-        <v>0</v>
-      </c>
-      <c r="P46" s="3"/>
-      <c r="Q46" s="5">
+      <c r="I46" s="8" t="b">
+        <v>0</v>
+      </c>
+      <c r="J46" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="K46" s="8">
+        <v>0</v>
+      </c>
+      <c r="L46" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="M46" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="N46" s="10">
+        <v>0</v>
+      </c>
+      <c r="O46" s="10">
+        <f>Table1[[#This Row],[Losses '[ratio'](%)]]*1000000</f>
+        <v>0</v>
+      </c>
+      <c r="P46" s="11">
+        <v>0</v>
+      </c>
+      <c r="Q46" s="8"/>
+      <c r="R46" s="10">
         <v>112987005</v>
       </c>
-      <c r="R46" s="5">
+      <c r="S46" s="10">
         <v>15692</v>
       </c>
-      <c r="S46" s="5">
+      <c r="T46" s="10">
         <v>125536</v>
       </c>
-      <c r="T46" s="2">
+      <c r="U46" s="7">
         <v>8159.84</v>
       </c>
-      <c r="U46" s="2">
+      <c r="V46" s="7">
         <v>8194.9900799999996</v>
       </c>
-      <c r="V46" s="5">
+      <c r="W46" s="10">
         <v>-1527965057</v>
       </c>
-      <c r="W46" s="3"/>
-    </row>
-    <row r="47" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="X46" s="8"/>
+    </row>
+    <row r="47" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A47" s="2">
         <v>7199.9649890000001</v>
       </c>
@@ -3787,50 +4034,75 @@
       <c r="N47" s="5">
         <v>16</v>
       </c>
-      <c r="O47" s="6">
+      <c r="O47" s="5">
+        <f>Table1[[#This Row],[Losses '[ratio'](%)]]*1000000</f>
+        <v>0.11640041296829499</v>
+      </c>
+      <c r="P47" s="6">
         <v>1.16400412968295E-7</v>
       </c>
-      <c r="P47" s="3" t="s">
+      <c r="Q47" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="Q47" s="5">
+      <c r="R47" s="5">
         <v>137456557</v>
       </c>
-      <c r="R47" s="5">
+      <c r="S47" s="5">
         <v>19091</v>
       </c>
-      <c r="S47" s="5">
+      <c r="T47" s="5">
         <v>152728</v>
       </c>
-      <c r="T47" s="2">
+      <c r="U47" s="2">
         <v>9927.32</v>
       </c>
-      <c r="U47" s="2">
+      <c r="V47" s="2">
         <v>9970.0838399999993</v>
       </c>
-      <c r="V47" s="5">
+      <c r="W47" s="5">
         <v>-1552436484</v>
       </c>
-      <c r="W47" s="3"/>
-    </row>
-    <row r="51" spans="16:17" x14ac:dyDescent="0.2">
+      <c r="X47" s="3"/>
+    </row>
+    <row r="51" spans="16:19" x14ac:dyDescent="0.2">
       <c r="P51">
-        <f>N47+N43+N37+N36+N34</f>
-        <v>51</v>
+        <f>N47+N43+N37+N36+N34+N40+N41</f>
+        <v>68</v>
       </c>
       <c r="Q51">
-        <f>Q34+Q36+Q37+Q40+Q41+Q43+Q47</f>
+        <f>R34+R36+R37+R40+R41+R43+R47</f>
         <v>899711553</v>
       </c>
-    </row>
-    <row r="52" spans="16:17" x14ac:dyDescent="0.2">
-      <c r="P52">
+      <c r="S51">
+        <f>R34+R37+R36+R40+R41+R43+R46+R47</f>
+        <v>1012698558</v>
+      </c>
+    </row>
+    <row r="52" spans="16:19" x14ac:dyDescent="0.2">
+      <c r="P52" s="13">
         <f>P51/Q51</f>
-        <v>5.6684833967003647E-8</v>
+        <v>7.557977862267153E-8</v>
+      </c>
+    </row>
+    <row r="54" spans="16:19" x14ac:dyDescent="0.2">
+      <c r="P54">
+        <f>N42+N45</f>
+        <v>8598</v>
+      </c>
+      <c r="Q54">
+        <f>R44+R45+R46+R42+R38+R39+R35+R33</f>
+        <v>900398584</v>
+      </c>
+    </row>
+    <row r="55" spans="16:19" x14ac:dyDescent="0.2">
+      <c r="P55" s="14">
+        <f>P54/Q54</f>
+        <v>9.5491043108970506E-6</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
   </tableParts>

</xml_diff>